<commit_message>
tentative 1 cache navigateur
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Titoune\Desktop\formation_open _classrooms\Avec_tuteur\Projets\P4_tristan_riedinger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F483376-B695-4073-B790-322C36EB5692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9E2DE7-0323-4A34-A1E7-83C8FEE1BAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>Catégorie</t>
   </si>
@@ -249,6 +249,21 @@
   </si>
   <si>
     <t>10) Reajuster les contrastes</t>
+  </si>
+  <si>
+    <t>Importance pour le référencement[modifier]</t>
+  </si>
+  <si>
+    <t>La réécriture et la réorientation des URL en particulier sont particulièrement importantes pour l’optimisation du référencement. Le statut de redirection est particulièrement important d’un point de vue du SEO. Si rien n’est spécifié, la plupart des serveurs interprètent cela comme une redirection temporaire et le considèrent comme un code de statut 302. Si la redirection doit être interprétée comme une redirection permanente (301), cela doit être cependant explicitement spécifié, car une redirection 301 transfère le classement de la source liée à la ressource cible.</t>
+  </si>
+  <si>
+    <t>Une redirection 302 est différemment interprétée par Google. Le renvoi est considéré comme temporaire et la réputation de la source liée n’est pas transférée à la ressource cible. Lors de la redirection ou de la réécriture d’URL, ainsi que de l’affectation à une ressource “www”, une redirection 301 doit être choisie.</t>
+  </si>
+  <si>
+    <t>La décision de rediriger vers une version “www” si une URL dépourvue de www est téléchargée est également importante, parce qu’une URL canonique aide Google dans l’identification de l’adresse par défaut. Le duplicate content est évité. Dans toutes les redirections, il est important de s’assurer qu’aucun code d’erreur 404 n’est généré. Google n’indexe normalement pas les sites qui affichent un code d’erreur 404 au serveur. Une gestion technique incorrecte des redirections via le htaccess peut avoir un impact majeur sur la réputation d’un site web, et entraîne parfois la désindexation de ce dernier ou encore son déclassement dans les SERP.</t>
+  </si>
+  <si>
+    <t>https://fr.ryte.com/wiki/Htaccess</t>
   </si>
 </sst>
 </file>
@@ -649,8 +664,8 @@
   <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1072,37 +1087,52 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
+      <c r="B33" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
+      <c r="C34" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
+      <c r="C35" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
+      <c r="C36" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
+      <c r="C37" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>

</xml_diff>